<commit_message>
new input files generation for english version; make only 20 different versions and duplicate many times for 1000 subjects
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2.2_english/input_files/100_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2.2_english/input_files/100_scenecat_block_order.xlsx
@@ -360,22 +360,22 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>living_rooms_1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>bedrooms_1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>kitchens_1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>kitchens_2</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>living_rooms_1</t>
+          <t>living_rooms_2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -385,16 +385,16 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>living_rooms_2</t>
+          <t>kitchens_2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -417,16 +417,16 @@
         <v>0</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -474,10 +474,10 @@
         <v>0</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>